<commit_message>
Agile Time keeper Q&A
</commit_message>
<xml_diff>
--- a/SQA Training Plan/SQA Training Plan.xlsx
+++ b/SQA Training Plan/SQA Training Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AG Training_Ateeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AG Training_Ateeb\SQA Training Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFEF617-0C22-407C-9477-695A40E18552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367188A1-A122-4CE7-8873-C22792D7E8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="579" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>S.No.</t>
   </si>
@@ -1169,6 +1169,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1249,27 +1270,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1620,8 +1620,8 @@
   </sheetPr>
   <dimension ref="A1:AB977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1634,14 +1634,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1686,14 +1686,14 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="96">
+      <c r="A3" s="69">
         <v>0</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="91" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="66"/>
+      <c r="D3" s="75"/>
       <c r="E3" s="29" t="s">
         <v>8</v>
       </c>
@@ -1724,10 +1724,10 @@
       <c r="AB3" s="1"/>
     </row>
     <row r="4" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="83"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="67"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="30" t="s">
         <v>51</v>
       </c>
@@ -1758,10 +1758,10 @@
       <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="83"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="67"/>
+      <c r="D5" s="76"/>
       <c r="E5" s="30" t="s">
         <v>10</v>
       </c>
@@ -1796,10 +1796,10 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="B6" s="83"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="67"/>
+      <c r="D6" s="76"/>
       <c r="E6" s="30" t="s">
         <v>11</v>
       </c>
@@ -1834,10 +1834,10 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:28" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="97"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="68"/>
+      <c r="D7" s="77"/>
       <c r="E7" s="31" t="s">
         <v>35</v>
       </c>
@@ -1871,10 +1871,10 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28" ht="39" x14ac:dyDescent="0.25">
-      <c r="A8" s="98">
+      <c r="A8" s="71">
         <v>1</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="93" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12"/>
@@ -1913,8 +1913,8 @@
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="1:28" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="33" t="s">
@@ -1951,8 +1951,8 @@
       <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:28" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
-      <c r="B10" s="86"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="34" t="s">
@@ -1989,10 +1989,10 @@
       <c r="AB10" s="1"/>
     </row>
     <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="101">
+      <c r="A11" s="74">
         <v>2</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="93" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="12"/>
@@ -2031,8 +2031,8 @@
       <c r="AB11" s="1"/>
     </row>
     <row r="12" spans="1:28" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="97"/>
-      <c r="B12" s="85"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="35" t="s">
@@ -2067,10 +2067,10 @@
       <c r="AB12" s="1"/>
     </row>
     <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75">
+      <c r="A13" s="84">
         <v>3</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="81" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="15"/>
@@ -2078,7 +2078,9 @@
       <c r="E13" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="55"/>
+      <c r="F13" s="55" t="s">
+        <v>59</v>
+      </c>
       <c r="G13" s="41" t="s">
         <v>21</v>
       </c>
@@ -2105,8 +2107,8 @@
       <c r="AB13" s="1"/>
     </row>
     <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="16"/>
       <c r="D14" s="13"/>
       <c r="E14" s="36" t="s">
@@ -2137,8 +2139,8 @@
       <c r="AB14" s="1"/>
     </row>
     <row r="15" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="73"/>
+      <c r="A15" s="85"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="16"/>
       <c r="D15" s="13"/>
       <c r="E15" s="37" t="s">
@@ -2171,8 +2173,8 @@
       <c r="AB15" s="1"/>
     </row>
     <row r="16" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
-      <c r="B16" s="74"/>
+      <c r="A16" s="86"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="16"/>
       <c r="D16" s="14"/>
       <c r="E16" s="38" t="s">
@@ -2205,10 +2207,10 @@
       <c r="AB16" s="1"/>
     </row>
     <row r="17" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="75">
+      <c r="A17" s="84">
         <v>4</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="87" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="12"/>
@@ -2243,8 +2245,8 @@
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="76"/>
-      <c r="B18" s="79"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="88"/>
       <c r="C18" s="13"/>
       <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
@@ -2277,8 +2279,8 @@
       <c r="AB18" s="1"/>
     </row>
     <row r="19" spans="1:28" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="76"/>
-      <c r="B19" s="79"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="13"/>
       <c r="D19" s="17"/>
       <c r="E19" s="8" t="s">
@@ -2311,14 +2313,14 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="89">
+      <c r="A20" s="98">
         <v>5</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="96" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="18"/>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="78" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -2351,10 +2353,10 @@
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="97"/>
       <c r="C21" s="19"/>
-      <c r="D21" s="70"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="38" t="s">
         <v>41</v>
       </c>
@@ -2385,10 +2387,10 @@
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="90"/>
-      <c r="B22" s="88"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="97"/>
       <c r="C22" s="19"/>
-      <c r="D22" s="70"/>
+      <c r="D22" s="79"/>
       <c r="E22" s="38" t="s">
         <v>17</v>
       </c>
@@ -2419,10 +2421,10 @@
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="90"/>
-      <c r="B23" s="88"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="97"/>
       <c r="C23" s="19"/>
-      <c r="D23" s="70"/>
+      <c r="D23" s="79"/>
       <c r="E23" s="38" t="s">
         <v>18</v>
       </c>
@@ -2451,10 +2453,10 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="91"/>
-      <c r="B24" s="92"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="101"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="71"/>
+      <c r="D24" s="80"/>
       <c r="E24" s="39" t="s">
         <v>25</v>
       </c>
@@ -2483,14 +2485,14 @@
       <c r="AB24" s="1"/>
     </row>
     <row r="25" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="80">
+      <c r="A25" s="89">
         <v>6</v>
       </c>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="96" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="66" t="s">
+      <c r="D25" s="75" t="s">
         <v>30</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -2523,10 +2525,10 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
-      <c r="B26" s="88"/>
+      <c r="A26" s="90"/>
+      <c r="B26" s="97"/>
       <c r="C26" s="22"/>
-      <c r="D26" s="67"/>
+      <c r="D26" s="76"/>
       <c r="E26" s="38" t="s">
         <v>41</v>
       </c>
@@ -2557,10 +2559,10 @@
       <c r="AB26" s="1"/>
     </row>
     <row r="27" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
-      <c r="B27" s="88"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="67"/>
+      <c r="D27" s="76"/>
       <c r="E27" s="40" t="s">
         <v>17</v>
       </c>
@@ -2591,10 +2593,10 @@
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
-      <c r="B28" s="88"/>
+      <c r="A28" s="90"/>
+      <c r="B28" s="97"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="67"/>
+      <c r="D28" s="76"/>
       <c r="E28" s="40" t="s">
         <v>31</v>
       </c>
@@ -2623,10 +2625,10 @@
       <c r="AB28" s="1"/>
     </row>
     <row r="29" spans="1:28" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="81"/>
-      <c r="B29" s="88"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="97"/>
       <c r="C29" s="22"/>
-      <c r="D29" s="67"/>
+      <c r="D29" s="76"/>
       <c r="E29" s="26" t="s">
         <v>32</v>
       </c>
@@ -31102,6 +31104,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A8:A10"/>
@@ -31118,8 +31122,6 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>